<commit_message>
changed â€™ to '
</commit_message>
<xml_diff>
--- a/api/recommendations.xlsx
+++ b/api/recommendations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unionbankphilippines.sharepoint.com/sites/DataScienceInsightsTeam/Shared Documents/Projects/220217-UBP-Intelligent newsletter/Intermediate results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jecxell Mamangon\Downloads\Unionbank\articles-recommender\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C69FA45-BF5C-4C0F-B9AF-3D5AB59C1665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4452F0D-8AEC-48FD-A40C-6D5B39842BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Solving human and societal challenges the real drivers behind innovation</t>
   </si>
   <si>
-    <t xml:space="preserve"> The pace of technology innovation is growing ever faster, and we are starting to see wider adoption and applications for emerging technologies such as artificial intelligence (AI) and quantum computing . Fujitsu developed the worldâ€™s #1 supercomputer, Fugaku, jointly developed with RIKEN, and is also leading with our digital annealing service .</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -143,12 +140,6 @@
     <t>https://www.eenews.net/articles/europes-clean-energy-plan-has-a-mining-problem/</t>
   </si>
   <si>
-    <t>Europeâ€™s clean energy plan has a mining problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Europeâ€™s plan to slash Russian fossil fuel imports and accelerate renewable energy production will test its ability to mine or import the materials that are needed for clean energy technology, like copper, lithium and cobalt . It comes as supply chains strain against rising demand for renewable energy globally .</t>
-  </si>
-  <si>
     <t>https://www.business-standard.com/article/economy-policy/commercial-entities-reduce-electricity-bills-by-renewable-energy-mercom-122060600332_1.html</t>
   </si>
   <si>
@@ -164,9 +155,6 @@
     <t xml:space="preserve">Blockchain </t>
   </si>
   <si>
-    <t>CFOs canâ€™t avoid cryptoâ€”and 20% of large companies will use it in some way by 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Apple may finally be ordered to make chargers just like everyone else . Apple may have been ordered to produce chargers for the first time ever . Apple's iPhone and iPad line-in-the-line chargers can be used to charge the next generation of iPhones and iPads .</t>
   </si>
   <si>
@@ -185,9 +173,6 @@
     <t>Australian Mayor Proposes Paying Taxes in Cryptocurrency</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mayor of Gold Coast, Australia, has suggested that Australians could pay their local property taxes in cryptocurrency . Gold Coast Mayor Tom Tate sees crypto payments as a way to communicate Australiaâ€™s innovative virtue, effectively attracting young people . He also noted that the council will recruit a chief investment officer tasked with promoting â€œinnovation,â€ and looking into â€˜joint venturesâ€ involving the councilâ€™ï¿½s land .</t>
-  </si>
-  <si>
     <t>https://www.space.com/uranus-haze-neptune-layers-different-colors</t>
   </si>
   <si>
@@ -216,13 +201,28 @@
   </si>
   <si>
     <t xml:space="preserve"> EOS Space Systems has become a core partner for the SmartSat Co-operative Research Centre, becoming the 20th core partner alongside leading universities and global corporations . Project CHORUS aims to build on existing Australian technology in compact RF tactical terminals and optical communication to develop â€œleap-froggingâ€ technology that exploits bearer diversity .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The pace of technology innovation is growing ever faster, and we are starting to see wider adoption and applications for emerging technologies such as artificial intelligence (AI) and quantum computing . Fujitsu developed the world's #1 supercomputer, Fugaku, jointly developed with RIKEN, and is also leading with our digital annealing service .</t>
+  </si>
+  <si>
+    <t>Europe's clean energy plan has a mining problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Europe's plan to slash Russian fossil fuel imports and accelerate renewable energy production will test its ability to mine or import the materials that are needed for clean energy technology, like copper, lithium and cobalt . It comes as supply chains strain against rising demand for renewable energy globally .</t>
+  </si>
+  <si>
+    <t>CFOs can't avoid cryptoâ€”and 20% of large companies will use it in some way by 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mayor of Gold Coast, Australia, has suggested that Australians could pay their local property taxes in cryptocurrency . Gold Coast Mayor Tom Tate sees crypto payments as a way to communicate Australia's innovative virtue, effectively attracting young people . He also noted that the council will recruit a chief investment officer tasked with promoting â€œinnovation,â€ and looking into â€˜joint venturesâ€ involving the council'ï¿½s land .</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,21 +598,21 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.899999999999999">
+    <row r="1" spans="1:7" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -635,7 +635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="132.75" customHeight="1">
+    <row r="2" spans="1:7" ht="132.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -646,290 +646,290 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="210.75" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="201" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="201" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="255" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="255" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="159" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="173.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="173.25" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="173.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="173.25" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="171" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="216.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="216.75" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="212.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="C11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="212.25" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="153" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="192" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="209.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="153" customHeight="1">
-      <c r="A13" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="209.25" customHeight="1">
-      <c r="A14" s="4" t="s">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="141.75" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="145.5" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -966,79 +966,79 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>0</v>
       </c>
@@ -1049,12 +1049,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9c17ea00-afc0-481e-a5b3-1a7196d4e145" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0e4bcfb3-7e48-4390-a5e8-6ec6a03be2dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1295,24 +1297,48 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9c17ea00-afc0-481e-a5b3-1a7196d4e145" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0e4bcfb3-7e48-4390-a5e8-6ec6a03be2dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44D54216-CF6B-4381-B5E1-C8C61D2B9B7F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AD39079-B537-48ED-9737-BD1F0315203D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c17ea00-afc0-481e-a5b3-1a7196d4e145"/>
+    <ds:schemaRef ds:uri="0e4bcfb3-7e48-4390-a5e8-6ec6a03be2dd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C59CEFF-EB02-4A85-9E50-C772B30403C8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C59CEFF-EB02-4A85-9E50-C772B30403C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0e4bcfb3-7e48-4390-a5e8-6ec6a03be2dd"/>
+    <ds:schemaRef ds:uri="9c17ea00-afc0-481e-a5b3-1a7196d4e145"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AD39079-B537-48ED-9737-BD1F0315203D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44D54216-CF6B-4381-B5E1-C8C61D2B9B7F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>